<commit_message>
Implemented Sheet read functionality for insert scripts
</commit_message>
<xml_diff>
--- a/DbScript/dbConfig/Enrollment/PersonNameActual/structure.xlsx
+++ b/DbScript/dbConfig/Enrollment/PersonNameActual/structure.xlsx
@@ -5,18 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Piyali\Tasks\Short_Term_Goal\TestdataGenerationTool\TestDataGen\DbScript\dbConfig\Enrollment\PersonNameActual\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaydutt\source\test\TestDataGen\DbScript\dbConfig\Enrollment\PersonNameActual\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFAD31B6-F464-48B4-8BD5-E4DAED117A02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17FB3A62-BA90-40AB-A9BC-A7916336FD0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="structure" sheetId="1" r:id="rId1"/>
-    <sheet name="insert" sheetId="2" r:id="rId2"/>
-    <sheet name="update" sheetId="3" r:id="rId3"/>
-    <sheet name="delete" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="24">
   <si>
     <t>columnname</t>
   </si>
@@ -97,6 +94,9 @@
   </si>
   <si>
     <t>lowercasealphanumeric</t>
+  </si>
+  <si>
+    <t>Sheet</t>
   </si>
 </sst>
 </file>
@@ -119,18 +119,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -197,34 +191,33 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -513,175 +506,175 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38" style="2" customWidth="1"/>
-    <col min="5" max="5" width="14.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="7.77734375" style="2"/>
+    <col min="1" max="1" width="16.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38" style="1" customWidth="1"/>
+    <col min="5" max="5" width="14.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="7.77734375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="8" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2">
         <v>3</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="J2" s="9" t="s">
+      <c r="J2" s="8" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <v>10</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="7"/>
-      <c r="I3" s="8" t="s">
+      <c r="H3" s="6"/>
+      <c r="I3" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="J3" s="9" t="s">
+      <c r="J3" s="8" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="2">
         <v>10</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="H4" s="7"/>
-      <c r="I4" s="8" t="s">
+      <c r="H4" s="6"/>
+      <c r="I4" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="J4" s="9" t="s">
+      <c r="J4" s="8" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
         <v>10</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="7"/>
-      <c r="I5" s="8" t="s">
+      <c r="H5" s="6"/>
+      <c r="I5" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="J5" s="9" t="s">
+      <c r="J5" s="8" t="s">
         <v>9</v>
       </c>
     </row>
@@ -699,109 +692,4 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17047232-4086-45AC-BEDA-C9D99AB94054}">
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD308740-176E-4F07-A897-5EE4CC607C5F}">
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{447DF1FE-625D-4B4B-8C80-77E3900CC4B9}">
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>